<commit_message>
Modified .gitignore and license overview
</commit_message>
<xml_diff>
--- a/LicenseOverview.xlsx
+++ b/LicenseOverview.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Library</t>
   </si>
@@ -172,6 +172,16 @@
   </si>
   <si>
     <t xml:space="preserve"> - Library for simple formatting of data to make it more human readable
+ - Included as Dll, code is available on the project's homepage</t>
+  </si>
+  <si>
+    <t>OpenXmlSdk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/OfficeDev/Open-XML-SDK </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Library for working with OpenXML file 
  - Included as Dll, code is available on the project's homepage</t>
   </si>
 </sst>
@@ -605,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,6 +826,20 @@
         <v>45</v>
       </c>
     </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -830,8 +854,9 @@
     <hyperlink ref="C12" r:id="rId10"/>
     <hyperlink ref="C13" r:id="rId11"/>
     <hyperlink ref="C14" r:id="rId12"/>
+    <hyperlink ref="C15" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a StraightMoveAnimation for 3D-Cameras
</commit_message>
<xml_diff>
--- a/LicenseOverview.xlsx
+++ b/LicenseOverview.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Library</t>
   </si>
@@ -182,6 +182,16 @@
   </si>
   <si>
     <t xml:space="preserve"> - Library for working with OpenXML file 
+ - Included as Dll, code is available on the project's homepage</t>
+  </si>
+  <si>
+    <t>Json.Net</t>
+  </si>
+  <si>
+    <t>http://www.newtonsoft.com/json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Library for serialization/deserialization into/from json format
  - Included as Dll, code is available on the project's homepage</t>
   </si>
 </sst>
@@ -615,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,6 +848,20 @@
       </c>
       <c r="D15" s="8" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -855,8 +879,9 @@
     <hyperlink ref="C13" r:id="rId11"/>
     <hyperlink ref="C14" r:id="rId12"/>
     <hyperlink ref="C15" r:id="rId13"/>
+    <hyperlink ref="C16" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Seeing#: Removed old SeeingSharp.MainProjects.sln
</commit_message>
<xml_diff>
--- a/LicenseOverview.xlsx
+++ b/LicenseOverview.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\RolandKoenig\FrozenSky\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10848"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10845"/>
   </bookViews>
   <sheets>
     <sheet name="Verwendete Lizenzen" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Library</t>
   </si>
@@ -47,9 +42,6 @@
     <t>PropertyTools</t>
   </si>
   <si>
-    <t>ZXing</t>
-  </si>
-  <si>
     <t>Reactive Extensions</t>
   </si>
   <si>
@@ -81,9 +73,6 @@
   </si>
   <si>
     <t>https://github.com/objorke/PropertyTools</t>
-  </si>
-  <si>
-    <t>http://code.google.com/p/zxing/</t>
   </si>
   <si>
     <t>https://rx.codeplex.com/license</t>
@@ -130,10 +119,6 @@
   <si>
     <t xml:space="preserve"> - Base classes for mathematics, including Vector3, Matrix, ...
  - Coding directly copied from SharpDX project and marked with ".MIT.cs"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Library for barcode processing
- - Included as Dll, code is available on the project's homepage</t>
   </si>
   <si>
     <t xml:space="preserve"> - Library for smart PropertyGrids in WPF
@@ -346,7 +331,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -617,7 +602,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -625,36 +610,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="9" customWidth="1"/>
     <col min="3" max="3" width="44" style="9" customWidth="1"/>
-    <col min="4" max="4" width="69.21875" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="5"/>
+    <col min="4" max="4" width="69.28515625" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="11.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -662,13 +647,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -676,13 +661,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -690,13 +675,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -704,13 +689,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -718,116 +703,116 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="D8" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>44</v>
@@ -836,32 +821,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>47</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -871,7 +842,7 @@
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId6"/>
     <hyperlink ref="C9" r:id="rId7"/>
     <hyperlink ref="C10" r:id="rId8"/>
     <hyperlink ref="C11" r:id="rId9"/>
@@ -879,9 +850,8 @@
     <hyperlink ref="C13" r:id="rId11"/>
     <hyperlink ref="C14" r:id="rId12"/>
     <hyperlink ref="C15" r:id="rId13"/>
-    <hyperlink ref="C16" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>